<commit_message>
Update scores for week X
</commit_message>
<xml_diff>
--- a/data/PointsScored_Survivor_48.xlsx
+++ b/data/PointsScored_Survivor_48.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsaacSchultz\Documents\Survivor_Python\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FE63E9-5989-4D58-B74E-A6FFD22598AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF0F031-682F-4016-AF44-FB4FC80CF0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DE998299-741F-409E-917F-4B7DAD429CF1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PointsScored_Survivor" sheetId="1" r:id="rId1"/>
@@ -445,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -458,7 +457,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -684,13 +682,12 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AO997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AF18" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="AL18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AJ27" sqref="AJ27"/>
+      <selection pane="bottomRight" activeCell="AO29" sqref="AO29"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -839,10 +836,10 @@
       <c r="AJ1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="10" t="s">
+      <c r="AK1" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="10" t="s">
+      <c r="AL1" s="9" t="s">
         <v>86</v>
       </c>
       <c r="AM1" t="s">
@@ -1041,7 +1038,7 @@
       <c r="A18" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18">
         <v>2</v>
       </c>
       <c r="AH18" s="1"/>
@@ -1051,7 +1048,7 @@
       <c r="A19" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19">
         <v>2</v>
       </c>
       <c r="AH19" s="1"/>
@@ -1063,7 +1060,7 @@
       <c r="A20" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20">
         <v>2</v>
       </c>
       <c r="AH20" s="1"/>
@@ -1076,7 +1073,7 @@
       <c r="A21" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21">
         <v>2</v>
       </c>
     </row>
@@ -1084,7 +1081,7 @@
       <c r="A22" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22">
         <v>2</v>
       </c>
     </row>
@@ -1092,7 +1089,7 @@
       <c r="A23" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23">
         <v>2</v>
       </c>
     </row>
@@ -1100,7 +1097,7 @@
       <c r="A24" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24">
         <v>2</v>
       </c>
       <c r="AH24" s="1"/>
@@ -1109,7 +1106,7 @@
       <c r="A25" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25">
         <v>2</v>
       </c>
       <c r="AH25" s="1"/>
@@ -1121,7 +1118,7 @@
       <c r="A26" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26">
         <v>2</v>
       </c>
     </row>
@@ -1129,7 +1126,7 @@
       <c r="A27" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27">
         <v>2</v>
       </c>
       <c r="AI27" s="1"/>
@@ -1138,7 +1135,7 @@
       <c r="A28" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28">
         <v>2</v>
       </c>
       <c r="AH28" s="1"/>
@@ -1150,7 +1147,7 @@
       <c r="A29" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29">
         <v>2</v>
       </c>
       <c r="AG29" s="1"/>
@@ -1160,7 +1157,7 @@
       <c r="A30" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30">
         <v>2</v>
       </c>
       <c r="L30" s="1"/>
@@ -1170,7 +1167,7 @@
       <c r="A31" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31">
         <v>2</v>
       </c>
       <c r="AG31" s="1"/>
@@ -1183,7 +1180,7 @@
       <c r="A32" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32">
         <v>2</v>
       </c>
       <c r="AG32" s="1"/>
@@ -2422,9 +2419,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2437,147 +2431,147 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>53</v>
       </c>
       <c r="C6" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="9" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2593,9 +2587,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="L19" sqref="L19"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="S32" sqref="S32"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2629,10 +2620,10 @@
       <c r="C2" s="1">
         <v>3</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2">
         <v>2</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2">
         <v>1</v>
       </c>
     </row>
@@ -2649,7 +2640,7 @@
       <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3">
         <v>0</v>
       </c>
     </row>
@@ -3683,14 +3674,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABC1FEC-B626-46F0-AE97-C498D904E4E1}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3725,7 +3712,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3751,14 +3738,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>81</v>
       </c>
       <c r="D3" t="b">
@@ -3777,14 +3764,14 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>72</v>
       </c>
       <c r="D4" t="b">
@@ -3803,7 +3790,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3829,7 +3816,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3868,16 +3855,16 @@
       <c r="D7" t="b">
         <v>0</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="11" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3926,7 +3913,7 @@
       <c r="F9" t="s">
         <v>75</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="12" t="s">
         <v>72</v>
       </c>
       <c r="H9" t="s">
@@ -3972,16 +3959,16 @@
       <c r="D11" t="b">
         <v>0</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="11" t="s">
         <v>59</v>
       </c>
     </row>
@@ -4012,13 +3999,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H12" xr:uid="{3ABC1FEC-B626-46F0-AE97-C498D904E4E1}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="2"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H12" xr:uid="{3ABC1FEC-B626-46F0-AE97-C498D904E4E1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4030,7 +4011,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Update scores week 3
</commit_message>
<xml_diff>
--- a/data/PointsScored_Survivor_48.xlsx
+++ b/data/PointsScored_Survivor_48.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsaacSchultz\Documents\Survivor_Python\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3221DF6-6BA7-433A-898D-16F0D2E29BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37219F34-1683-41C1-A9C8-4F0EA47B37D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PointsScored_Survivor" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,10 @@
     <sheet name="Elimination_Table" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PointsScored_Survivor!$A$1:$AJ$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PointsScored_Survivor!$A$1:$AJ$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Weekly_Questions!$A$1:$H$12</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="y+UqypyAIi4+2xqziDClQ4BPr2IEqJD/nCAXQZ95ZFE="/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="94">
   <si>
     <t>Player</t>
   </si>
@@ -303,6 +303,18 @@
   </si>
   <si>
     <t>Plays idol at tribal</t>
+  </si>
+  <si>
+    <t>Plays advantage (extra vote, steal vote etc.)</t>
+  </si>
+  <si>
+    <t>Will there be a journey?</t>
+  </si>
+  <si>
+    <t>Will Sai go Goblin mode?</t>
+  </si>
+  <si>
+    <t>Week 3</t>
   </si>
 </sst>
 </file>
@@ -444,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -464,6 +476,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,13 +692,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO997"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:AP996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AF33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AO1" sqref="AO1"/>
+      <selection pane="bottomRight" activeCell="AF54" sqref="AF54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -724,9 +738,10 @@
     <col min="39" max="39" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="40.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -850,8 +865,11 @@
       <c r="AO1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -862,7 +880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -873,7 +891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -882,7 +900,7 @@
       </c>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -892,7 +910,7 @@
       <c r="L5" s="1"/>
       <c r="AJ5" s="1"/>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -903,7 +921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -914,7 +932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -928,7 +946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -937,7 +955,7 @@
       </c>
       <c r="AI9" s="1"/>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -948,7 +966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -957,7 +975,7 @@
       </c>
       <c r="AI11" s="1"/>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -968,7 +986,7 @@
       <c r="AI12" s="1"/>
       <c r="AJ12" s="1"/>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -985,7 +1003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -1002,7 +1020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -1011,7 +1029,7 @@
       </c>
       <c r="AH15" s="1"/>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -1022,7 +1040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -1033,7 +1051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -1043,7 +1061,7 @@
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
     </row>
-    <row r="19" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:42" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -1055,7 +1073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:42" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1067,8 +1085,11 @@
       <c r="AO20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AP20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -1076,7 +1097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:42" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -1084,7 +1105,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:42" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -1092,7 +1113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:42" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -1101,7 +1122,7 @@
       </c>
       <c r="AH24" s="1"/>
     </row>
-    <row r="25" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:42" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -1113,7 +1134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:42" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -1121,7 +1142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:42" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -1130,7 +1151,7 @@
       </c>
       <c r="AI27" s="1"/>
     </row>
-    <row r="28" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:42" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -1142,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -1152,7 +1173,7 @@
       <c r="AG29" s="1"/>
       <c r="AH29" s="1"/>
     </row>
-    <row r="30" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -1162,7 +1183,7 @@
       <c r="L30" s="1"/>
       <c r="AG30" s="1"/>
     </row>
-    <row r="31" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:42" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -1175,7 +1196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:42" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -1187,187 +1208,278 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
+    <row r="33" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
       <c r="U33" s="1"/>
       <c r="AG33" s="1"/>
-      <c r="AH33" s="1"/>
-    </row>
-    <row r="34" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
+      <c r="AH33" s="9"/>
+      <c r="AI33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="AH34" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ34" s="9"/>
+    </row>
+    <row r="35" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
       <c r="AG35" s="1"/>
-    </row>
-    <row r="36" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
+      <c r="AH35" s="9"/>
+      <c r="AI35">
+        <v>1</v>
+      </c>
+      <c r="AJ35" s="9"/>
+    </row>
+    <row r="36" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
       <c r="AG36" s="1"/>
-      <c r="AH36" s="1"/>
-    </row>
-    <row r="37" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
+      <c r="AH36" s="9"/>
+      <c r="AJ36" s="9"/>
+    </row>
+    <row r="37" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
       <c r="AG37" s="1"/>
-      <c r="AH37" s="1"/>
-    </row>
-    <row r="38" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
+      <c r="AH37" s="9"/>
+      <c r="AJ37" s="9"/>
+    </row>
+    <row r="38" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
       <c r="AG38" s="1"/>
-    </row>
-    <row r="39" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
+      <c r="AI38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
       <c r="AG39" s="1"/>
-    </row>
-    <row r="40" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
+      <c r="AI39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
       <c r="AG40" s="1"/>
-    </row>
-    <row r="41" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
+      <c r="AH40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
       <c r="AH41" s="1"/>
     </row>
-    <row r="42" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="AH42" s="1"/>
-    </row>
-    <row r="43" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="AH43" s="1"/>
-    </row>
-    <row r="44" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-    </row>
-    <row r="45" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-    </row>
-    <row r="46" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="V46" s="1"/>
-    </row>
-    <row r="47" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="AG42" s="9"/>
+      <c r="AH42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="AG43" s="9"/>
+    </row>
+    <row r="44" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="AG44" s="9"/>
+    </row>
+    <row r="45" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="V45" s="1"/>
+      <c r="AG45" s="9"/>
+      <c r="AH45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="AG46" s="9"/>
+      <c r="AH46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
+      <c r="L47" s="1"/>
       <c r="AH47" s="1"/>
     </row>
-    <row r="48" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
-      <c r="L48" s="1"/>
       <c r="AH48" s="1"/>
     </row>
-    <row r="49" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
-      <c r="AH49" s="1"/>
-    </row>
-    <row r="50" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L49" s="1"/>
+    </row>
+    <row r="50" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
-      <c r="L50" s="1"/>
-    </row>
-    <row r="51" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
     </row>
-    <row r="52" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
-    </row>
-    <row r="53" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB52" s="1"/>
+    </row>
+    <row r="53" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
-      <c r="AB53" s="1"/>
-    </row>
-    <row r="54" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
-    </row>
-    <row r="55" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W54" s="1"/>
+    </row>
+    <row r="55" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
-      <c r="W55" s="1"/>
-    </row>
-    <row r="56" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
-    </row>
-    <row r="57" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W56" s="1"/>
+    </row>
+    <row r="57" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
-      <c r="W57" s="1"/>
-    </row>
-    <row r="58" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
     </row>
-    <row r="59" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
     </row>
-    <row r="60" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
-    </row>
-    <row r="61" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M60" s="1"/>
+    </row>
+    <row r="61" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
-      <c r="M61" s="1"/>
-    </row>
-    <row r="62" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
     </row>
-    <row r="63" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
-    </row>
-    <row r="64" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC63" s="1"/>
+    </row>
+    <row r="64" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
-      <c r="AC64" s="1"/>
+      <c r="AJ64" s="1"/>
     </row>
     <row r="65" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
-      <c r="AJ65" s="1"/>
+      <c r="AH65" s="1"/>
     </row>
     <row r="66" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
-      <c r="AH66" s="1"/>
     </row>
     <row r="67" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
+      <c r="AJ67" s="1"/>
     </row>
     <row r="68" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
-      <c r="AJ68" s="1"/>
+      <c r="AH68" s="1"/>
     </row>
     <row r="69" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
-      <c r="AH69" s="1"/>
+      <c r="AJ69" s="1"/>
     </row>
     <row r="70" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
-      <c r="AJ70" s="1"/>
+      <c r="AH70" s="1"/>
     </row>
     <row r="71" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
@@ -1377,22 +1489,21 @@
     <row r="72" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
-      <c r="AH72" s="1"/>
     </row>
     <row r="73" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
+      <c r="Y73" s="1"/>
+      <c r="AH73" s="1"/>
     </row>
     <row r="74" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
-      <c r="Y74" s="1"/>
       <c r="AH74" s="1"/>
     </row>
     <row r="75" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
-      <c r="AH75" s="1"/>
     </row>
     <row r="76" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
@@ -1405,12 +1516,12 @@
     <row r="78" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
+      <c r="Y78" s="1"/>
+      <c r="AH78" s="1"/>
     </row>
     <row r="79" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
-      <c r="Y79" s="1"/>
-      <c r="AH79" s="1"/>
     </row>
     <row r="80" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
@@ -1419,16 +1530,16 @@
     <row r="81" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
+      <c r="AH81" s="1"/>
     </row>
     <row r="82" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
-      <c r="AH82" s="1"/>
+      <c r="K82" s="1"/>
     </row>
     <row r="83" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
-      <c r="K83" s="1"/>
     </row>
     <row r="84" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
@@ -1445,11 +1556,11 @@
     <row r="87" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
+      <c r="J87" s="1"/>
     </row>
     <row r="88" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
-      <c r="J88" s="1"/>
     </row>
     <row r="89" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
@@ -1458,17 +1569,17 @@
     <row r="90" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
+      <c r="Y90" s="1"/>
+      <c r="AJ90" s="1"/>
     </row>
     <row r="91" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
-      <c r="Y91" s="1"/>
-      <c r="AJ91" s="1"/>
+      <c r="AH91" s="1"/>
     </row>
     <row r="92" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
-      <c r="AH92" s="1"/>
     </row>
     <row r="93" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
@@ -1477,11 +1588,11 @@
     <row r="94" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
+      <c r="I94" s="1"/>
     </row>
     <row r="95" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
-      <c r="I95" s="1"/>
     </row>
     <row r="96" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
@@ -1494,12 +1605,9 @@
     <row r="98" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
-    </row>
-    <row r="99" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="Y99" s="1"/>
-    </row>
+      <c r="Y98" s="1"/>
+    </row>
+    <row r="99" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="100" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="101" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="102" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2397,9 +2505,14 @@
     <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:AJ32" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AJ46" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="3"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -2410,7 +2523,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2476,9 +2589,7 @@
       <c r="F4" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>47</v>
-      </c>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
@@ -2578,7 +2689,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2638,10 +2749,21 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="13">
+        <v>3</v>
+      </c>
+      <c r="E4" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -3667,10 +3789,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABC1FEC-B626-46F0-AE97-C498D904E4E1}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3989,6 +4111,188 @@
       </c>
       <c r="H12" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -4002,7 +4306,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4053,8 +4357,12 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>

</xml_diff>

<commit_message>
Fixed standings chart to include bonus points
</commit_message>
<xml_diff>
--- a/data/PointsScored_Survivor_48.xlsx
+++ b/data/PointsScored_Survivor_48.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsaacSchultz\Documents\Survivor_Python\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB11EBF7-CE7F-4B29-9085-0E5B80290403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04790E77-9EE0-433B-883A-E0D206AEB8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PointsScored_Survivor" sheetId="1" r:id="rId1"/>
@@ -695,10 +695,10 @@
   <dimension ref="A1:AP996"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AH4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AH14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AK20" sqref="AK20"/>
+      <selection pane="bottomRight" activeCell="AI56" sqref="AI56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -890,7 +890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -931,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:42" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:42" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:42" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1233,7 +1233,7 @@
       </c>
       <c r="AJ34" s="9"/>
     </row>
-    <row r="35" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:36" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:36" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:36" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -2508,8 +2508,7 @@
   <autoFilter ref="A1:AJ46" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="Kamilla"/>
-        <filter val="Kyle"/>
+        <filter val="Bianca"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2523,7 +2522,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2688,8 +2687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3791,8 +3790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABC1FEC-B626-46F0-AE97-C498D904E4E1}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4306,7 +4305,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Week 9 and 10 scores
</commit_message>
<xml_diff>
--- a/data/PointsScored_Survivor_48.xlsx
+++ b/data/PointsScored_Survivor_48.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsaacSchultz\Documents\Survivor_Python\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB0F386-F668-4545-9A04-62BC4A66AF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51EAAB2-7FF9-4970-8079-C882E291B930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A549BF43-C147-4A07-BF22-B3F340E87A7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tribes" sheetId="6" r:id="rId1"/>
@@ -20,8 +21,8 @@
     <sheet name="Elimination_Table" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PointsScored_Survivor!$A$1:$AK$98</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Weekly_Questions!$A$1:$H$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PointsScored_Survivor!$A$1:$AK$111</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Weekly_Questions!$A$1:$H$73</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="142">
   <si>
     <t>Player</t>
   </si>
@@ -434,17 +435,60 @@
   </si>
   <si>
     <t>Week 8</t>
+  </si>
+  <si>
+    <t>Week 9</t>
+  </si>
+  <si>
+    <t>Week 10</t>
+  </si>
+  <si>
+    <t>Who will say the ep title "Coconut Etiquette"?</t>
+  </si>
+  <si>
+    <t>Will anyone play anything at tribal?</t>
+  </si>
+  <si>
+    <t>Reward challenge?</t>
+  </si>
+  <si>
+    <t>Will anyone from strong boys be eliminated?</t>
+  </si>
+  <si>
+    <t>Who will say the ep title "Icarus Time"?</t>
+  </si>
+  <si>
+    <t>One person chosen to join reward</t>
+  </si>
+  <si>
+    <t>Anyone discuss actually voting for Eva?</t>
+  </si>
+  <si>
+    <t>Will Mitch or Kamilla be murked?</t>
+  </si>
+  <si>
+    <t>Will Kamilla and Kyle vote together?</t>
+  </si>
+  <si>
+    <t>Will Kamilla and Kyle break up?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -572,31 +616,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -815,8 +858,9 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -978,14 +1022,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:AV990"/>
+  <dimension ref="A1:AV988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="U82" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AN89" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V104" sqref="V104"/>
+      <selection pane="bottomRight" activeCell="AR110" sqref="AR110"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <pane xSplit="1" topLeftCell="AM1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AM108" sqref="AM108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1027,6 +1074,7 @@
     <col min="43" max="43" width="40.42578125" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="26" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.25">
@@ -1175,7 +1223,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1186,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1197,7 +1245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1206,7 +1254,7 @@
       </c>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1216,7 +1264,7 @@
       <c r="M5" s="1"/>
       <c r="AK5" s="1"/>
     </row>
-    <row r="6" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1227,7 +1275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -1238,7 +1286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1252,7 +1300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1261,7 +1309,7 @@
       </c>
       <c r="AJ9" s="1"/>
     </row>
-    <row r="10" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1272,7 +1320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -1281,7 +1329,7 @@
       </c>
       <c r="AJ11" s="1"/>
     </row>
-    <row r="12" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -1292,7 +1340,7 @@
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1"/>
     </row>
-    <row r="13" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1309,7 +1357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -1326,7 +1374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -1335,7 +1383,7 @@
       </c>
       <c r="AI15" s="1"/>
     </row>
-    <row r="16" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -1346,7 +1394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -1357,7 +1405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1367,7 +1415,7 @@
       <c r="AI18" s="1"/>
       <c r="AJ18" s="1"/>
     </row>
-    <row r="19" spans="1:43" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -1379,7 +1427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:43" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1395,7 +1443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:43" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1403,7 +1451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:43" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -1411,7 +1459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:43" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -1419,7 +1467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:43" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1428,7 +1476,7 @@
       </c>
       <c r="AI24" s="1"/>
     </row>
-    <row r="25" spans="1:43" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1440,7 +1488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:43" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -1448,7 +1496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:43" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -1457,7 +1505,7 @@
       </c>
       <c r="AJ27" s="1"/>
     </row>
-    <row r="28" spans="1:43" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -1469,7 +1517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:43" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1479,7 +1527,7 @@
       <c r="AH29" s="1"/>
       <c r="AI29" s="1"/>
     </row>
-    <row r="30" spans="1:43" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -1489,7 +1537,7 @@
       <c r="M30" s="1"/>
       <c r="AH30" s="1"/>
     </row>
-    <row r="31" spans="1:43" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -1502,7 +1550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:43" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -1514,7 +1562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:45" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -1528,7 +1576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:45" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -1540,7 +1588,7 @@
       </c>
       <c r="AK34" s="9"/>
     </row>
-    <row r="35" spans="1:45" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1554,7 +1602,7 @@
       </c>
       <c r="AK35" s="9"/>
     </row>
-    <row r="36" spans="1:45" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -1565,7 +1613,7 @@
       <c r="AI36" s="9"/>
       <c r="AK36" s="9"/>
     </row>
-    <row r="37" spans="1:45" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -1576,7 +1624,7 @@
       <c r="AI37" s="9"/>
       <c r="AK37" s="9"/>
     </row>
-    <row r="38" spans="1:45" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -1588,7 +1636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:45" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -1600,7 +1648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:45" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -1612,7 +1660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:45" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -1621,7 +1669,7 @@
       </c>
       <c r="AI41" s="1"/>
     </row>
-    <row r="42" spans="1:45" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>55</v>
       </c>
@@ -1633,7 +1681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:45" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -1642,7 +1690,7 @@
       </c>
       <c r="AH43" s="9"/>
     </row>
-    <row r="44" spans="1:45" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>57</v>
       </c>
@@ -1651,7 +1699,7 @@
       </c>
       <c r="AH44" s="9"/>
     </row>
-    <row r="45" spans="1:45" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -1664,7 +1712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:45" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>59</v>
       </c>
@@ -1676,7 +1724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:45" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -1695,7 +1743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:45" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1707,7 +1755,7 @@
       </c>
       <c r="AI48" s="1"/>
     </row>
-    <row r="49" spans="1:47" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -1725,7 +1773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:47" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1736,7 +1784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:47" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1750,7 +1798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:47" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1765,7 +1813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:47" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1782,7 +1830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:47" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1797,7 +1845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:47" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1808,7 +1856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:47" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -1820,7 +1868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:47" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -1834,7 +1882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:47" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -1848,7 +1896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:47" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -1863,7 +1911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:47" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>47</v>
       </c>
@@ -1874,7 +1922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:47" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>48</v>
       </c>
@@ -1882,7 +1930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:47" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>35</v>
       </c>
@@ -1894,7 +1942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:47" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>49</v>
       </c>
@@ -1906,7 +1954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:47" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>50</v>
       </c>
@@ -1915,7 +1963,7 @@
       </c>
       <c r="AI64" s="1"/>
     </row>
-    <row r="65" spans="1:39" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>51</v>
       </c>
@@ -1929,7 +1977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:39" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>52</v>
       </c>
@@ -1938,7 +1986,7 @@
       </c>
       <c r="AK66" s="1"/>
     </row>
-    <row r="67" spans="1:39" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>53</v>
       </c>
@@ -1952,7 +2000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:39" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>54</v>
       </c>
@@ -1964,7 +2012,7 @@
       </c>
       <c r="AK68" s="1"/>
     </row>
-    <row r="69" spans="1:39" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>57</v>
       </c>
@@ -1973,7 +2021,7 @@
       </c>
       <c r="AI69" s="1"/>
     </row>
-    <row r="70" spans="1:39" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>58</v>
       </c>
@@ -1981,7 +2029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:39" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>59</v>
       </c>
@@ -1993,7 +2041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:39" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>47</v>
       </c>
@@ -2005,7 +2053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:39" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>48</v>
       </c>
@@ -2019,7 +2067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:39" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>35</v>
       </c>
@@ -2030,7 +2078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:39" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>49</v>
       </c>
@@ -2041,7 +2089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:39" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>51</v>
       </c>
@@ -2052,7 +2100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:39" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>52</v>
       </c>
@@ -2063,7 +2111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:39" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>53</v>
       </c>
@@ -2074,7 +2122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:39" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>57</v>
       </c>
@@ -2088,7 +2136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:39" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>58</v>
       </c>
@@ -2102,7 +2150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:48" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>59</v>
       </c>
@@ -2272,7 +2320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>58</v>
       </c>
@@ -2283,7 +2331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>59</v>
       </c>
@@ -2291,23 +2339,141 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="12"/>
-      <c r="B99" s="1"/>
-    </row>
-    <row r="100" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>47</v>
+      </c>
+      <c r="B99">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>48</v>
+      </c>
+      <c r="B100">
+        <v>9</v>
+      </c>
+      <c r="AK100">
+        <v>1</v>
+      </c>
+      <c r="AV100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>35</v>
+      </c>
+      <c r="B101">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="102" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>49</v>
+      </c>
+      <c r="B102">
+        <v>9</v>
+      </c>
+      <c r="AV102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>51</v>
+      </c>
+      <c r="B103">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>52</v>
+      </c>
+      <c r="B104">
+        <v>9</v>
+      </c>
+      <c r="Z104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>59</v>
+      </c>
+      <c r="B105">
+        <v>9</v>
+      </c>
+      <c r="I105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>47</v>
+      </c>
+      <c r="B106">
+        <v>10</v>
+      </c>
+      <c r="H106">
+        <v>1</v>
+      </c>
+      <c r="AI106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>48</v>
+      </c>
+      <c r="B107">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>35</v>
+      </c>
+      <c r="B108">
+        <v>10</v>
+      </c>
+      <c r="AV108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>49</v>
+      </c>
+      <c r="B109">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>51</v>
+      </c>
+      <c r="B110">
+        <v>10</v>
+      </c>
+      <c r="Z110">
+        <v>1</v>
+      </c>
+      <c r="AV110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>52</v>
+      </c>
+      <c r="B111">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3184,17 +3350,8 @@
     <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:AK98" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="7"/>
-        <filter val="8"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AK111" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -3204,9 +3361,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3359,11 +3517,45 @@
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9">
         <v>5</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9">
         <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4355,11 +4547,12 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABC1FEC-B626-46F0-AE97-C498D904E4E1}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E59" sqref="E59:H59"/>
+      <selection activeCell="O75" sqref="O75:O76"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5620,7 +5813,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>7</v>
       </c>
@@ -5646,7 +5839,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>7</v>
       </c>
@@ -5672,7 +5865,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>8</v>
       </c>
@@ -5685,20 +5878,20 @@
       <c r="D51" t="b">
         <v>0</v>
       </c>
-      <c r="E51" s="15" t="s">
+      <c r="E51" t="s">
         <v>35</v>
       </c>
-      <c r="F51" s="15" t="s">
+      <c r="F51" t="s">
         <v>59</v>
       </c>
-      <c r="G51" s="13" t="s">
+      <c r="G51" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="H51" s="16" t="s">
+      <c r="H51" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>8</v>
       </c>
@@ -5711,20 +5904,20 @@
       <c r="D52" t="b">
         <v>0</v>
       </c>
-      <c r="E52" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F52" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G52" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H52" s="16" t="s">
+      <c r="E52" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G52" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H52" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>8</v>
       </c>
@@ -5737,20 +5930,20 @@
       <c r="D53" t="b">
         <v>0</v>
       </c>
-      <c r="E53" s="13" t="s">
+      <c r="E53" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F53" s="13" t="s">
+      <c r="F53" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G53" s="13" t="s">
+      <c r="G53" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H53" s="17" t="s">
+      <c r="H53" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>8</v>
       </c>
@@ -5763,20 +5956,20 @@
       <c r="D54" t="b">
         <v>0</v>
       </c>
-      <c r="E54" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F54" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="G54" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="H54" s="17" t="s">
+      <c r="E54" t="s">
+        <v>41</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G54" t="s">
+        <v>41</v>
+      </c>
+      <c r="H54" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>8</v>
       </c>
@@ -5789,20 +5982,20 @@
       <c r="D55" t="b">
         <v>0</v>
       </c>
-      <c r="E55" s="13" t="s">
+      <c r="E55" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F55" s="16" t="s">
+      <c r="F55" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G55" s="15" t="s">
+      <c r="G55" t="s">
         <v>35</v>
       </c>
-      <c r="H55" s="17" t="s">
+      <c r="H55" s="13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>8</v>
       </c>
@@ -5815,20 +6008,20 @@
       <c r="D56" t="b">
         <v>0</v>
       </c>
-      <c r="E56" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F56" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="G56" s="13" t="s">
+      <c r="E56" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G56" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H56" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H56" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>8</v>
       </c>
@@ -5841,20 +6034,20 @@
       <c r="D57" t="b">
         <v>0</v>
       </c>
-      <c r="E57" s="17" t="s">
+      <c r="E57" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F57" s="17" t="s">
+      <c r="F57" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="G57" s="13" t="s">
+      <c r="G57" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H57" s="17" t="s">
+      <c r="H57" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>8</v>
       </c>
@@ -5867,27 +6060,432 @@
       <c r="D58" t="b">
         <v>0</v>
       </c>
-      <c r="E58" s="17" t="s">
+      <c r="E58" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="F58" s="16" t="s">
+      <c r="F58" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="G58" s="15" t="s">
+      <c r="G58" t="s">
         <v>49</v>
       </c>
-      <c r="H58" s="16" t="s">
+      <c r="H58" s="12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G60" s="14"/>
+    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>9</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D59" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H59" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="K59">
+        <v>9</v>
+      </c>
+      <c r="L59">
+        <v>1</v>
+      </c>
+      <c r="M59">
+        <v>2</v>
+      </c>
+      <c r="N59">
+        <v>3</v>
+      </c>
+      <c r="O59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>9</v>
+      </c>
+      <c r="B60" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D60" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K60">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>9</v>
+      </c>
+      <c r="B61" t="s">
+        <v>133</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D61" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F61" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H61" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>9</v>
+      </c>
+      <c r="B62" t="s">
+        <v>134</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D62" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G62" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H62" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>9</v>
+      </c>
+      <c r="B63" t="s">
+        <v>141</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D63" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F63" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>9</v>
+      </c>
+      <c r="B64" t="s">
+        <v>135</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D64" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>9</v>
+      </c>
+      <c r="B65" t="s">
+        <v>69</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D65" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>10</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C66" t="s">
+        <v>47</v>
+      </c>
+      <c r="D66" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F66" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G66" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H66" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>10</v>
+      </c>
+      <c r="B67" t="s">
+        <v>94</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D67" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F67" t="s">
+        <v>47</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H67" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>10</v>
+      </c>
+      <c r="B68" t="s">
+        <v>90</v>
+      </c>
+      <c r="C68" t="s">
+        <v>40</v>
+      </c>
+      <c r="D68" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>10</v>
+      </c>
+      <c r="B69" t="s">
+        <v>137</v>
+      </c>
+      <c r="C69" t="s">
+        <v>35</v>
+      </c>
+      <c r="D69" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F69" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>10</v>
+      </c>
+      <c r="B70" t="s">
+        <v>138</v>
+      </c>
+      <c r="C70" t="s">
+        <v>41</v>
+      </c>
+      <c r="D70" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G70" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>10</v>
+      </c>
+      <c r="B71" t="s">
+        <v>139</v>
+      </c>
+      <c r="C71" t="s">
+        <v>40</v>
+      </c>
+      <c r="D71" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F71" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>10</v>
+      </c>
+      <c r="B72" t="s">
+        <v>140</v>
+      </c>
+      <c r="C72" t="s">
+        <v>41</v>
+      </c>
+      <c r="D72" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F72" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G72" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H72" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>10</v>
+      </c>
+      <c r="B73" t="s">
+        <v>69</v>
+      </c>
+      <c r="C73" t="s">
+        <v>47</v>
+      </c>
+      <c r="D73" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H58" xr:uid="{3ABC1FEC-B626-46F0-AE97-C498D904E4E1}">
+  <autoFilter ref="A1:H73" xr:uid="{3ABC1FEC-B626-46F0-AE97-C498D904E4E1}">
     <filterColumn colId="0">
       <filters>
-        <filter val="8"/>
+        <filter val="10"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -5899,9 +6497,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6007,11 +6606,20 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>

</xml_diff>

<commit_message>
Week 9 and 10 scores again
</commit_message>
<xml_diff>
--- a/data/PointsScored_Survivor_48.xlsx
+++ b/data/PointsScored_Survivor_48.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsaacSchultz\Documents\Survivor_Python\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51EAAB2-7FF9-4970-8079-C882E291B930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6BFF99-F993-4873-9F17-E29A04FDB2C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A549BF43-C147-4A07-BF22-B3F340E87A7B}"/>
   </bookViews>
   <sheets>
@@ -567,7 +567,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -588,44 +588,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -873,145 +843,145 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="7" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C6" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="7" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1189,10 +1159,10 @@
       <c r="AK1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="AL1" s="9" t="s">
+      <c r="AL1" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="AM1" s="9" t="s">
+      <c r="AM1" s="7" t="s">
         <v>85</v>
       </c>
       <c r="AN1" t="s">
@@ -1571,7 +1541,7 @@
       </c>
       <c r="V33" s="1"/>
       <c r="AH33" s="1"/>
-      <c r="AI33" s="9"/>
+      <c r="AI33" s="7"/>
       <c r="AJ33">
         <v>1</v>
       </c>
@@ -1583,10 +1553,10 @@
       <c r="B34">
         <v>3</v>
       </c>
-      <c r="AI34" s="9">
-        <v>1</v>
-      </c>
-      <c r="AK34" s="9"/>
+      <c r="AI34" s="7">
+        <v>1</v>
+      </c>
+      <c r="AK34" s="7"/>
     </row>
     <row r="35" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1596,11 +1566,11 @@
         <v>3</v>
       </c>
       <c r="AH35" s="1"/>
-      <c r="AI35" s="9"/>
+      <c r="AI35" s="7"/>
       <c r="AJ35">
         <v>1</v>
       </c>
-      <c r="AK35" s="9"/>
+      <c r="AK35" s="7"/>
     </row>
     <row r="36" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -1610,8 +1580,8 @@
         <v>3</v>
       </c>
       <c r="AH36" s="1"/>
-      <c r="AI36" s="9"/>
-      <c r="AK36" s="9"/>
+      <c r="AI36" s="7"/>
+      <c r="AK36" s="7"/>
     </row>
     <row r="37" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -1621,8 +1591,8 @@
         <v>3</v>
       </c>
       <c r="AH37" s="1"/>
-      <c r="AI37" s="9"/>
-      <c r="AK37" s="9"/>
+      <c r="AI37" s="7"/>
+      <c r="AK37" s="7"/>
     </row>
     <row r="38" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -1676,7 +1646,7 @@
       <c r="B42">
         <v>3</v>
       </c>
-      <c r="AH42" s="9"/>
+      <c r="AH42" s="7"/>
       <c r="AI42" s="1">
         <v>1</v>
       </c>
@@ -1688,7 +1658,7 @@
       <c r="B43">
         <v>3</v>
       </c>
-      <c r="AH43" s="9"/>
+      <c r="AH43" s="7"/>
     </row>
     <row r="44" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -1697,7 +1667,7 @@
       <c r="B44">
         <v>3</v>
       </c>
-      <c r="AH44" s="9"/>
+      <c r="AH44" s="7"/>
     </row>
     <row r="45" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -1707,7 +1677,7 @@
         <v>3</v>
       </c>
       <c r="W45" s="1"/>
-      <c r="AH45" s="9"/>
+      <c r="AH45" s="7"/>
       <c r="AI45">
         <v>1</v>
       </c>
@@ -1719,7 +1689,7 @@
       <c r="B46">
         <v>3</v>
       </c>
-      <c r="AH46" s="9"/>
+      <c r="AH46" s="7"/>
       <c r="AI46" s="1">
         <v>1</v>
       </c>
@@ -2246,7 +2216,7 @@
       </c>
     </row>
     <row r="90" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="12" t="s">
+      <c r="A90" s="10" t="s">
         <v>53</v>
       </c>
       <c r="B90" s="1">
@@ -3361,8 +3331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -3372,7 +3342,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -3381,10 +3351,10 @@
       <c r="C1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3508,7 +3478,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="A9" s="10">
         <v>8</v>
       </c>
       <c r="B9">
@@ -3525,7 +3495,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
+      <c r="A10" s="12">
         <v>9</v>
       </c>
       <c r="B10">
@@ -3542,7 +3512,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
+      <c r="A11" s="12">
         <v>10</v>
       </c>
       <c r="B11">
@@ -4546,11 +4516,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABC1FEC-B626-46F0-AE97-C498D904E4E1}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:O73"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O75" sqref="O75:O76"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -4591,7 +4560,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4617,14 +4586,14 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>80</v>
       </c>
       <c r="D3" t="b">
@@ -4643,14 +4612,14 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>71</v>
       </c>
       <c r="D4" t="b">
@@ -4669,7 +4638,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4695,7 +4664,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4721,7 +4690,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -4747,7 +4716,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -4773,14 +4742,14 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D9" t="b">
@@ -4799,14 +4768,14 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>80</v>
       </c>
       <c r="D10" t="b">
@@ -4825,14 +4794,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D11" t="b">
@@ -4851,14 +4820,14 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D12" t="b">
@@ -4877,14 +4846,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
       <c r="B13" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="3" t="s">
         <v>76</v>
       </c>
       <c r="D13" t="b">
@@ -4903,14 +4872,14 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
       <c r="B14" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D14" t="b">
@@ -4929,14 +4898,14 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
       <c r="B15" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D15" t="b">
@@ -4955,7 +4924,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -4981,7 +4950,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -5007,7 +4976,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -5033,7 +5002,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3</v>
       </c>
@@ -5059,7 +5028,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
@@ -5085,7 +5054,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -5111,7 +5080,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4</v>
       </c>
@@ -5137,7 +5106,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4</v>
       </c>
@@ -5163,7 +5132,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4</v>
       </c>
@@ -5189,7 +5158,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4</v>
       </c>
@@ -5215,7 +5184,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4</v>
       </c>
@@ -5241,7 +5210,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4</v>
       </c>
@@ -5267,7 +5236,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5</v>
       </c>
@@ -5293,7 +5262,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>5</v>
       </c>
@@ -5306,10 +5275,10 @@
       <c r="D29" t="b">
         <v>0</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="9" t="s">
         <v>53</v>
       </c>
       <c r="G29" t="s">
@@ -5319,7 +5288,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5</v>
       </c>
@@ -5332,20 +5301,20 @@
       <c r="D30" t="b">
         <v>0</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="9" t="s">
         <v>40</v>
       </c>
       <c r="F30" t="s">
         <v>41</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="G30" s="9" t="s">
         <v>40</v>
       </c>
       <c r="H30" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5</v>
       </c>
@@ -5358,20 +5327,20 @@
       <c r="D31" t="b">
         <v>0</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="9" t="s">
         <v>40</v>
       </c>
       <c r="F31" t="s">
         <v>41</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="9" t="s">
         <v>40</v>
       </c>
       <c r="H31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>5</v>
       </c>
@@ -5397,7 +5366,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>5</v>
       </c>
@@ -5423,7 +5392,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>5</v>
       </c>
@@ -5436,20 +5405,20 @@
       <c r="D34" t="b">
         <v>0</v>
       </c>
-      <c r="E34" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H34" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E34" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>5</v>
       </c>
@@ -5465,7 +5434,7 @@
       <c r="E35" t="s">
         <v>35</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F35" s="9" t="s">
         <v>50</v>
       </c>
       <c r="G35" t="s">
@@ -5475,7 +5444,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>6</v>
       </c>
@@ -5494,14 +5463,14 @@
       <c r="F36" t="s">
         <v>49</v>
       </c>
-      <c r="G36" s="11" t="s">
+      <c r="G36" s="9" t="s">
         <v>51</v>
       </c>
       <c r="H36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>6</v>
       </c>
@@ -5527,7 +5496,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>6</v>
       </c>
@@ -5553,7 +5522,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>6</v>
       </c>
@@ -5579,7 +5548,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>6</v>
       </c>
@@ -5605,7 +5574,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>6</v>
       </c>
@@ -5631,7 +5600,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>6</v>
       </c>
@@ -5644,7 +5613,7 @@
       <c r="D42" t="b">
         <v>0</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="9" t="s">
         <v>57</v>
       </c>
       <c r="F42" t="s">
@@ -5653,11 +5622,11 @@
       <c r="G42" t="s">
         <v>49</v>
       </c>
-      <c r="H42" s="11" t="s">
+      <c r="H42" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>7</v>
       </c>
@@ -5670,10 +5639,10 @@
       <c r="D43" t="b">
         <v>0</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="E43" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F43" s="11" t="s">
+      <c r="F43" s="9" t="s">
         <v>47</v>
       </c>
       <c r="G43" t="s">
@@ -5683,7 +5652,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>7</v>
       </c>
@@ -5709,7 +5678,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>7</v>
       </c>
@@ -5722,20 +5691,20 @@
       <c r="D45" t="b">
         <v>0</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="E45" s="9" t="s">
         <v>40</v>
       </c>
       <c r="F45" t="s">
         <v>41</v>
       </c>
-      <c r="G45" s="11" t="s">
+      <c r="G45" s="9" t="s">
         <v>40</v>
       </c>
       <c r="H45" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>7</v>
       </c>
@@ -5748,20 +5717,20 @@
       <c r="D46" t="b">
         <v>0</v>
       </c>
-      <c r="E46" s="11" t="s">
+      <c r="E46" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F46" s="11" t="s">
+      <c r="F46" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G46" s="11" t="s">
+      <c r="G46" s="9" t="s">
         <v>40</v>
       </c>
       <c r="H46" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>7</v>
       </c>
@@ -5774,20 +5743,20 @@
       <c r="D47" t="b">
         <v>0</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="E47" s="9" t="s">
         <v>40</v>
       </c>
       <c r="F47" t="s">
         <v>41</v>
       </c>
-      <c r="G47" s="11" t="s">
+      <c r="G47" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H47" s="11" t="s">
+      <c r="H47" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>7</v>
       </c>
@@ -5806,14 +5775,14 @@
       <c r="F48" t="s">
         <v>49</v>
       </c>
-      <c r="G48" s="11" t="s">
+      <c r="G48" s="9" t="s">
         <v>51</v>
       </c>
       <c r="H48" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>7</v>
       </c>
@@ -5829,17 +5798,17 @@
       <c r="E49" t="s">
         <v>49</v>
       </c>
-      <c r="F49" s="11" t="s">
+      <c r="F49" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="G49" s="11" t="s">
+      <c r="G49" s="9" t="s">
         <v>53</v>
       </c>
       <c r="H49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>7</v>
       </c>
@@ -5852,27 +5821,27 @@
       <c r="D50" t="b">
         <v>0</v>
       </c>
-      <c r="E50" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G50" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H50" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E50" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>8</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B51" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C51" s="10" t="s">
         <v>58</v>
       </c>
       <c r="D51" t="b">
@@ -5884,73 +5853,73 @@
       <c r="F51" t="s">
         <v>59</v>
       </c>
-      <c r="G51" s="11" t="s">
+      <c r="G51" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H51" s="12" t="s">
+      <c r="H51" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>8</v>
       </c>
       <c r="B52" t="s">
         <v>111</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C52" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D52" t="b">
         <v>0</v>
       </c>
-      <c r="E52" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F52" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G52" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H52" s="12" t="s">
+      <c r="E52" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H52" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>8</v>
       </c>
       <c r="B53" t="s">
         <v>90</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="10" t="s">
         <v>40</v>
       </c>
       <c r="D53" t="b">
         <v>0</v>
       </c>
-      <c r="E53" s="11" t="s">
+      <c r="E53" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F53" s="11" t="s">
+      <c r="F53" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G53" s="11" t="s">
+      <c r="G53" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H53" s="13" t="s">
+      <c r="H53" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>8</v>
       </c>
       <c r="B54" t="s">
         <v>125</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C54" s="10" t="s">
         <v>40</v>
       </c>
       <c r="D54" t="b">
@@ -5959,317 +5928,299 @@
       <c r="E54" t="s">
         <v>41</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="F54" s="10" t="s">
         <v>41</v>
       </c>
       <c r="G54" t="s">
         <v>41</v>
       </c>
-      <c r="H54" s="13" t="s">
+      <c r="H54" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>8</v>
       </c>
       <c r="B55" t="s">
         <v>94</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C55" s="10" t="s">
         <v>51</v>
       </c>
       <c r="D55" t="b">
         <v>0</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="E55" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F55" s="12" t="s">
+      <c r="F55" s="10" t="s">
         <v>35</v>
       </c>
       <c r="G55" t="s">
         <v>35</v>
       </c>
-      <c r="H55" s="13" t="s">
+      <c r="H55" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>8</v>
       </c>
       <c r="B56" t="s">
         <v>126</v>
       </c>
-      <c r="C56" s="12" t="s">
+      <c r="C56" s="10" t="s">
         <v>40</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
       </c>
-      <c r="E56" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F56" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G56" s="11" t="s">
+      <c r="E56" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G56" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H56" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H56" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>8</v>
       </c>
       <c r="B57" t="s">
         <v>127</v>
       </c>
-      <c r="C57" s="12" t="s">
+      <c r="C57" s="10" t="s">
         <v>40</v>
       </c>
       <c r="D57" t="b">
         <v>0</v>
       </c>
-      <c r="E57" s="13" t="s">
+      <c r="E57" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F57" s="13" t="s">
+      <c r="F57" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G57" s="11" t="s">
+      <c r="G57" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H57" s="13" t="s">
+      <c r="H57" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>8</v>
       </c>
       <c r="B58" t="s">
         <v>69</v>
       </c>
-      <c r="C58" s="12" t="s">
+      <c r="C58" s="10" t="s">
         <v>58</v>
       </c>
       <c r="D58" t="b">
         <v>0</v>
       </c>
-      <c r="E58" s="13" t="s">
+      <c r="E58" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F58" s="12" t="s">
+      <c r="F58" s="10" t="s">
         <v>59</v>
       </c>
       <c r="G58" t="s">
         <v>49</v>
       </c>
-      <c r="H58" s="12" t="s">
+      <c r="H58" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>9</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D59" t="b">
         <v>0</v>
       </c>
-      <c r="E59" s="16" t="s">
+      <c r="E59" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F59" s="11" t="s">
+      <c r="F59" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G59" s="5" t="s">
+      <c r="G59" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H59" s="12" t="s">
+      <c r="H59" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="K59">
-        <v>9</v>
-      </c>
-      <c r="L59">
-        <v>1</v>
-      </c>
-      <c r="M59">
-        <v>2</v>
-      </c>
-      <c r="N59">
-        <v>3</v>
-      </c>
-      <c r="O59">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>9</v>
       </c>
       <c r="B60" t="s">
         <v>94</v>
       </c>
-      <c r="C60" s="12" t="s">
+      <c r="C60" s="10" t="s">
         <v>52</v>
       </c>
       <c r="D60" t="b">
         <v>0</v>
       </c>
-      <c r="E60" s="16" t="s">
+      <c r="E60" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F60" s="5" t="s">
+      <c r="F60" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G60" s="5" t="s">
+      <c r="G60" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H60" s="5" t="s">
+      <c r="H60" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K60">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>9</v>
       </c>
       <c r="B61" t="s">
         <v>133</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C61" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D61" t="b">
         <v>0</v>
       </c>
-      <c r="E61" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F61" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H61" s="11" t="s">
+      <c r="E61" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F61" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H61" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>9</v>
       </c>
       <c r="B62" t="s">
         <v>134</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D62" t="b">
         <v>0</v>
       </c>
-      <c r="E62" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G62" s="11" t="s">
+      <c r="E62" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G62" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H62" s="11" t="s">
+      <c r="H62" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>9</v>
       </c>
       <c r="B63" t="s">
         <v>141</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C63" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
       </c>
-      <c r="E63" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F63" s="11" t="s">
+      <c r="E63" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F63" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G63" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H63" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G63" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>9</v>
       </c>
       <c r="B64" t="s">
         <v>135</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D64" t="b">
         <v>0</v>
       </c>
-      <c r="E64" s="15" t="s">
+      <c r="E64" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F64" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G64" s="11" t="s">
+      <c r="F64" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G64" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H64" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H64" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>9</v>
       </c>
       <c r="B65" t="s">
         <v>69</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="3" t="s">
         <v>59</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
       </c>
-      <c r="E65" s="16" t="s">
+      <c r="E65" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F65" s="5" t="s">
+      <c r="F65" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G65" s="11" t="s">
+      <c r="G65" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H65" s="5" t="s">
+      <c r="H65" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6277,7 +6228,7 @@
       <c r="A66">
         <v>10</v>
       </c>
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="12" t="s">
         <v>136</v>
       </c>
       <c r="C66" t="s">
@@ -6286,16 +6237,16 @@
       <c r="D66" t="b">
         <v>0</v>
       </c>
-      <c r="E66" s="11" t="s">
+      <c r="E66" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F66" s="11" t="s">
+      <c r="F66" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G66" s="11" t="s">
+      <c r="G66" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H66" s="11" t="s">
+      <c r="H66" s="9" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6306,22 +6257,22 @@
       <c r="B67" t="s">
         <v>94</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C67" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D67" t="b">
         <v>0</v>
       </c>
-      <c r="E67" s="16" t="s">
+      <c r="E67" s="14" t="s">
         <v>48</v>
       </c>
       <c r="F67" t="s">
         <v>47</v>
       </c>
-      <c r="G67" s="5" t="s">
+      <c r="G67" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H67" s="11" t="s">
+      <c r="H67" s="9" t="s">
         <v>51</v>
       </c>
     </row>
@@ -6338,16 +6289,16 @@
       <c r="D68" t="b">
         <v>0</v>
       </c>
-      <c r="E68" s="16" t="s">
+      <c r="E68" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F68" s="5" t="s">
+      <c r="F68" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G68" s="5" t="s">
+      <c r="G68" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H68" s="5" t="s">
+      <c r="H68" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -6364,16 +6315,16 @@
       <c r="D69" t="b">
         <v>0</v>
       </c>
-      <c r="E69" s="16" t="s">
+      <c r="E69" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F69" s="11" t="s">
+      <c r="F69" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G69" s="5" t="s">
+      <c r="G69" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H69" s="5" t="s">
+      <c r="H69" s="3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -6390,16 +6341,16 @@
       <c r="D70" t="b">
         <v>0</v>
       </c>
-      <c r="E70" s="16" t="s">
+      <c r="E70" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F70" s="5" t="s">
+      <c r="F70" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G70" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H70" s="5" t="s">
+      <c r="G70" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H70" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -6416,16 +6367,16 @@
       <c r="D71" t="b">
         <v>0</v>
       </c>
-      <c r="E71" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F71" s="11" t="s">
+      <c r="E71" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F71" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G71" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H71" s="5" t="s">
+      <c r="G71" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H71" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -6442,16 +6393,16 @@
       <c r="D72" t="b">
         <v>0</v>
       </c>
-      <c r="E72" s="16" t="s">
+      <c r="E72" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F72" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G72" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H72" s="11" t="s">
+      <c r="F72" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H72" s="9" t="s">
         <v>41</v>
       </c>
     </row>
@@ -6468,27 +6419,21 @@
       <c r="D73" t="b">
         <v>0</v>
       </c>
-      <c r="E73" s="16" t="s">
+      <c r="E73" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F73" s="5" t="s">
+      <c r="F73" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G73" s="5" t="s">
+      <c r="G73" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H73" s="5" t="s">
+      <c r="H73" s="3" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H73" xr:uid="{3ABC1FEC-B626-46F0-AE97-C498D904E4E1}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="10"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H73" xr:uid="{3ABC1FEC-B626-46F0-AE97-C498D904E4E1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6497,8 +6442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -6598,26 +6543,26 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="10" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="12" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="12" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>